<commit_message>
lagt til så vi ikke har ulovlige variabler
</commit_message>
<xml_diff>
--- a/data_generation/Parameterdata-sheets.xlsx
+++ b/data_generation/Parameterdata-sheets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/camillalie/Downloads/masteroppgave/data_generation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5682EF79-A5D9-BE45-83A7-E480EFC07465}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F14FAC-5D35-6F44-B868-650FBAB67450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3540" yWindow="780" windowWidth="30660" windowHeight="19700" firstSheet="4" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3540" yWindow="780" windowWidth="30660" windowHeight="19700" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cost of retrofitting" sheetId="1" r:id="rId1"/>
@@ -539,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" activeCellId="2" sqref="A8:XFD8 A12:XFD12 A16:XFD16"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -568,8 +568,8 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>1</v>
+      <c r="B2" s="1">
+        <v>2</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -583,7 +583,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -597,7 +597,7 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -607,130 +607,17 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7">
-        <v>7</v>
-      </c>
+      <c r="A5" s="1"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <v>2</v>
-      </c>
-      <c r="B8" s="1">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>7</v>
-      </c>
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>2</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>7</v>
-      </c>
+      <c r="A9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>2</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-      <c r="D10">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
-        <v>2</v>
-      </c>
-      <c r="B11" s="1">
-        <v>2</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>2</v>
-      </c>
-      <c r="B12">
-        <v>2</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>2</v>
-      </c>
-      <c r="B13">
-        <v>2</v>
-      </c>
-      <c r="C13">
-        <v>2</v>
-      </c>
-      <c r="D13">
-        <v>7</v>
-      </c>
+      <c r="A10" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6283,7 +6170,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6380,7 +6267,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6426,7 +6313,7 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -6437,7 +6324,7 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -6537,8 +6424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6701,10 +6588,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6728,7 +6615,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -6742,7 +6629,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -6755,42 +6642,42 @@
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4">
-        <v>0</v>
+      <c r="B4" s="1">
+        <v>1</v>
       </c>
       <c r="C4">
         <v>2</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>500</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
-      <c r="B5">
-        <v>1</v>
+      <c r="B5" s="1">
+        <v>2</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>500</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
-      <c r="B6">
-        <v>1</v>
+      <c r="B6" s="1">
+        <v>2</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>500</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -6798,7 +6685,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -6812,7 +6699,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -6826,7 +6713,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -6840,7 +6727,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -6854,7 +6741,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -6868,7 +6755,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -6882,7 +6769,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -6896,7 +6783,7 @@
         <v>1</v>
       </c>
       <c r="B14" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -6910,7 +6797,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -6924,7 +6811,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -6935,10 +6822,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>1</v>
-      </c>
-      <c r="B17" s="1">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -6949,10 +6836,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>1</v>
-      </c>
-      <c r="B18" s="1">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -6963,10 +6850,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B19" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -6979,50 +6866,50 @@
       <c r="A20">
         <v>2</v>
       </c>
-      <c r="B20">
-        <v>0</v>
+      <c r="B20" s="1">
+        <v>2</v>
       </c>
       <c r="C20">
         <v>0</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>500</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2</v>
       </c>
-      <c r="B21">
-        <v>0</v>
+      <c r="B21" s="1">
+        <v>2</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>500</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2</v>
       </c>
-      <c r="B22">
-        <v>0</v>
+      <c r="B22" s="1">
+        <v>2</v>
       </c>
       <c r="C22">
         <v>2</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>500</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2</v>
       </c>
-      <c r="B23">
-        <v>1</v>
+      <c r="B23" s="1">
+        <v>3</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -7035,8 +6922,8 @@
       <c r="A24">
         <v>2</v>
       </c>
-      <c r="B24">
-        <v>1</v>
+      <c r="B24" s="1">
+        <v>3</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -7050,7 +6937,7 @@
         <v>2</v>
       </c>
       <c r="B25" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C25">
         <v>2</v>
@@ -7064,7 +6951,7 @@
         <v>2</v>
       </c>
       <c r="B26" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -7078,7 +6965,7 @@
         <v>2</v>
       </c>
       <c r="B27" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -7092,7 +6979,7 @@
         <v>2</v>
       </c>
       <c r="B28" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C28">
         <v>2</v>
@@ -7106,7 +6993,7 @@
         <v>2</v>
       </c>
       <c r="B29" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -7120,7 +7007,7 @@
         <v>2</v>
       </c>
       <c r="B30" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -7134,96 +7021,12 @@
         <v>2</v>
       </c>
       <c r="B31" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C31">
         <v>2</v>
       </c>
       <c r="D31">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>2</v>
-      </c>
-      <c r="B32" s="1">
-        <v>4</v>
-      </c>
-      <c r="C32">
-        <v>0</v>
-      </c>
-      <c r="D32">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>2</v>
-      </c>
-      <c r="B33" s="1">
-        <v>4</v>
-      </c>
-      <c r="C33">
-        <v>1</v>
-      </c>
-      <c r="D33">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>2</v>
-      </c>
-      <c r="B34" s="1">
-        <v>4</v>
-      </c>
-      <c r="C34">
-        <v>2</v>
-      </c>
-      <c r="D34">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>2</v>
-      </c>
-      <c r="B35" s="1">
-        <v>5</v>
-      </c>
-      <c r="C35">
-        <v>0</v>
-      </c>
-      <c r="D35">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>2</v>
-      </c>
-      <c r="B36" s="1">
-        <v>5</v>
-      </c>
-      <c r="C36">
-        <v>1</v>
-      </c>
-      <c r="D36">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <v>2</v>
-      </c>
-      <c r="B37" s="1">
-        <v>5</v>
-      </c>
-      <c r="C37">
-        <v>2</v>
-      </c>
-      <c r="D37">
         <v>500</v>
       </c>
     </row>
@@ -7237,7 +7040,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7264,7 +7067,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>20</v>
+        <v>500</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -7275,7 +7078,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>20</v>
+        <v>500</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -7286,7 +7089,7 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>20</v>
+        <v>500</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -7297,7 +7100,7 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>40</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -7308,7 +7111,7 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>60</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -7319,7 +7122,7 @@
         <v>2</v>
       </c>
       <c r="C7">
-        <v>40</v>
+        <v>1000</v>
       </c>
     </row>
   </sheetData>
@@ -7331,8 +7134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K35" sqref="K35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7356,7 +7159,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>24.183168508800001</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -7367,7 +7170,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>16.339545988800001</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -7378,7 +7181,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>30.568922241599999</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -7389,7 +7192,7 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>0.3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -7400,7 +7203,7 @@
         <v>2</v>
       </c>
       <c r="C6">
-        <v>0.4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -7411,7 +7214,7 @@
         <v>3</v>
       </c>
       <c r="C7">
-        <v>0.2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -7424,7 +7227,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7448,7 +7251,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>23</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -7459,7 +7262,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>25</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -7470,7 +7273,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>30</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -7516,7 +7319,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D6"/>
+      <selection activeCell="C7" sqref="C7:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7546,7 +7349,7 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>23</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7560,7 +7363,7 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>25</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -7574,7 +7377,7 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <v>30</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -7630,8 +7433,7 @@
         <v>2</v>
       </c>
       <c r="D8">
-        <f>D2*0.75</f>
-        <v>17.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -7645,8 +7447,7 @@
         <v>2</v>
       </c>
       <c r="D9">
-        <f t="shared" ref="D9:D13" si="0">D3*0.75</f>
-        <v>18.75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -7660,8 +7461,7 @@
         <v>2</v>
       </c>
       <c r="D10">
-        <f t="shared" si="0"/>
-        <v>22.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -7675,7 +7475,7 @@
         <v>2</v>
       </c>
       <c r="D11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D11:D13" si="0">D5*0.75</f>
         <v>7.5</v>
       </c>
     </row>
@@ -7720,8 +7520,7 @@
         <v>3</v>
       </c>
       <c r="D14">
-        <f>D2*1.25</f>
-        <v>28.75</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -7735,8 +7534,7 @@
         <v>3</v>
       </c>
       <c r="D15">
-        <f t="shared" ref="D15:D19" si="1">D3*1.25</f>
-        <v>31.25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -7750,8 +7548,7 @@
         <v>3</v>
       </c>
       <c r="D16">
-        <f t="shared" si="1"/>
-        <v>37.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -7765,8 +7562,7 @@
         <v>3</v>
       </c>
       <c r="D17">
-        <f t="shared" si="1"/>
-        <v>12.5</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -7780,8 +7576,7 @@
         <v>3</v>
       </c>
       <c r="D18">
-        <f t="shared" si="1"/>
-        <v>18.75</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -7795,8 +7590,7 @@
         <v>3</v>
       </c>
       <c r="D19">
-        <f t="shared" si="1"/>
-        <v>6.25</v>
+        <v>10000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fikset data og sunsetvalue
</commit_message>
<xml_diff>
--- a/data_generation/Parameterdata-sheets.xlsx
+++ b/data_generation/Parameterdata-sheets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/camillalie/Downloads/masteroppgave/data_generation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F14FAC-5D35-6F44-B868-650FBAB67450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF7B5796-18FA-4E4B-825A-6FCE62CFF59E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3540" yWindow="780" windowWidth="30660" windowHeight="19700" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3540" yWindow="780" windowWidth="30660" windowHeight="19700" firstSheet="3" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cost of retrofitting" sheetId="1" r:id="rId1"/>
@@ -542,7 +542,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -603,7 +603,7 @@
         <v>2</v>
       </c>
       <c r="D4">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -6169,7 +6169,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -6207,7 +6207,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
   </sheetData>
@@ -6267,7 +6267,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6313,7 +6313,7 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -6357,7 +6357,7 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -6368,7 +6368,7 @@
         <v>1</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -6425,7 +6425,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6464,7 +6464,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -6472,7 +6472,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -6483,10 +6483,10 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -6499,7 +6499,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6588,10 +6588,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7028,6 +7028,146 @@
       </c>
       <c r="D31">
         <v>500</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32" s="1">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>3</v>
+      </c>
+      <c r="D32">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33" s="1">
+        <v>2</v>
+      </c>
+      <c r="C33">
+        <v>3</v>
+      </c>
+      <c r="D33">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>1</v>
+      </c>
+      <c r="B34" s="1">
+        <v>3</v>
+      </c>
+      <c r="C34">
+        <v>3</v>
+      </c>
+      <c r="D34">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35" s="1">
+        <v>4</v>
+      </c>
+      <c r="C35">
+        <v>3</v>
+      </c>
+      <c r="D35">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36" s="1">
+        <v>5</v>
+      </c>
+      <c r="C36">
+        <v>3</v>
+      </c>
+      <c r="D36">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>2</v>
+      </c>
+      <c r="B37" s="1">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>3</v>
+      </c>
+      <c r="D37">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>2</v>
+      </c>
+      <c r="B38" s="1">
+        <v>2</v>
+      </c>
+      <c r="C38">
+        <v>3</v>
+      </c>
+      <c r="D38">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>2</v>
+      </c>
+      <c r="B39" s="1">
+        <v>3</v>
+      </c>
+      <c r="C39">
+        <v>3</v>
+      </c>
+      <c r="D39">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>2</v>
+      </c>
+      <c r="B40" s="1">
+        <v>4</v>
+      </c>
+      <c r="C40">
+        <v>3</v>
+      </c>
+      <c r="D40">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>2</v>
+      </c>
+      <c r="B41" s="1">
+        <v>5</v>
+      </c>
+      <c r="C41">
+        <v>3</v>
+      </c>
+      <c r="D41">
+        <v>450</v>
       </c>
     </row>
   </sheetData>
@@ -7037,10 +7177,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7125,6 +7265,28 @@
         <v>1000</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>1000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7134,8 +7296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13647,10 +13809,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:C13"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13765,6 +13927,39 @@
         <v>1</v>
       </c>
     </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>